<commit_message>
small edits to Spanish translations
</commit_message>
<xml_diff>
--- a/scripts/LANGUAGES.xlsx
+++ b/scripts/LANGUAGES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/cowanm_who_int/Documents/R/GSHS/On Github/GSHS/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{8FD9F22F-2657-3440-9F80-7F28C7D047A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB05420-BFB9-4EAB-BCE7-0CE8EB367FC9}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{8FD9F22F-2657-3440-9F80-7F28C7D047A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CA029DC-4B72-4833-B341-BD54A83BADD8}"/>
   <bookViews>
-    <workbookView xWindow="31275" yWindow="0" windowWidth="25200" windowHeight="15300" xr2:uid="{9940F395-5CBF-1344-9EDE-5DC37C2C9B75}"/>
+    <workbookView xWindow="32115" yWindow="1125" windowWidth="21975" windowHeight="14475" xr2:uid="{9940F395-5CBF-1344-9EDE-5DC37C2C9B75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>c('Total','Âge (ans)','12 ans ou moins','13 - 15','16 ou 17','13 - 17','18 ans ou plus','Classe','Total' ,'Mâles','Femelles','Pourcentage','Intervalle\nde confiance\n à 95%','N')</t>
   </si>
   <si>
-    <t>c('Total','Edad (años)','12 años o menos','13 - 15','16 o 17','13 - 17','18 años o más','Clase',' Total','Hombres','Mujeres','Porcentaje','Intervalo \nde confianza \ndel 95%','N')</t>
-  </si>
-  <si>
     <t>c('Всего','Возраст (лет)','12 лет и младше','13–15','16 или 17','13–17','18 лет и старше','Оценка','Всего' ,'Мужчины','Женщины','Процент','95%\n доверительный \nинтервал','N')</t>
   </si>
   <si>
@@ -245,12 +242,6 @@
     <t>c('Общий')</t>
   </si>
   <si>
-    <t>c('Sin ponderar\nPorcentaje')</t>
-  </si>
-  <si>
-    <t>c('Ponderado\nPorcentaje')</t>
-  </si>
-  <si>
     <t>c('Hombres')</t>
   </si>
   <si>
@@ -260,9 +251,6 @@
     <t>c('Grado')</t>
   </si>
   <si>
-    <t>c('Nombre estándar\nVariable','País\nCuestionario\nNúmero','Pregunta\nCódigo y Etiqueta','Etiqueta','Sin ponderar\nFrecuencia','Sin ponderar\nPorcentaje')</t>
-  </si>
-  <si>
     <t>c('Edad (años)')</t>
   </si>
   <si>
@@ -272,17 +260,72 @@
     <t>c("Valor perdido")</t>
   </si>
   <si>
-    <t>c('Nombre estándar\nVariable','País\nCuestionario\nNúmero','Pregunta\nCódigo y Etiqueta','Etiqueta','Sin ponderar\nFrecuencia','Ponderado\nPorcentaje')</t>
-  </si>
-  <si>
     <t>c('Resultados de estudiantes de 13 a 17 años', 'Total', 'Hombres', 'Mujeres')</t>
+  </si>
+  <si>
+    <t>c('Porcentaje\nsin ponderar')</t>
+  </si>
+  <si>
+    <t>c('Porcentaje\nponderado')</t>
+  </si>
+  <si>
+    <r>
+      <t>c('</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nombre estándar\nvariable','Número\ncuestionario\npaís','Código y etiqueta\npregunta','Etiqueta','Frecuencia\nsin ponderar','Porcentaje\nponderado')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c('Total','Edad (años)','12 años o menos',</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'13-15','16 o 17','13-17','18 años o más','Clase',' Total','Hombres','Mujeres','Porcentaje','Intervalo \nde confianza \ndel 95%','N')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c('</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nombre estándar\nvariable','Número\ncuestionario\npaís','Código y etiqueta\npregunta','Etiqueta','Frecuencia\nsin ponderar','Porcentaje\nsin ponderar')</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,8 +354,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,10 +374,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +419,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +525,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -629,14 +677,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AD3873-7A4D-2546-9363-2286C47E6630}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="133.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="149.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="149.875" customWidth="1"/>
     <col min="3" max="3" width="149.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="154.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -655,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +713,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -682,8 +730,8 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>77</v>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -699,8 +747,8 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>78</v>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -716,11 +764,11 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -733,8 +781,8 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>75</v>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -750,7 +798,7 @@
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D7" t="s">
@@ -767,7 +815,7 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
@@ -784,7 +832,7 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
@@ -801,7 +849,7 @@
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D10" t="s">
@@ -818,7 +866,7 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
@@ -835,8 +883,8 @@
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>73</v>
+      <c r="C12" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -847,13 +895,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -864,19 +912,19 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>72</v>
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,8 +934,8 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>69</v>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
@@ -903,8 +951,8 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
-        <v>70</v>
+      <c r="C16" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -920,8 +968,8 @@
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
-        <v>76</v>
+      <c r="C17" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -932,19 +980,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -954,11 +1002,11 @@
       <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
@@ -966,56 +1014,375 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>54</v>
       </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2199b669-f139-4cad-81c0-f0198b00fad6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5e13aadc-de86-43ee-b386-40c01ba74c80" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067970A7EC1C90C48A386F8B78D31816E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c5a1f6eeb0442f3fe3a122bfaf1a852">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2199b669-f139-4cad-81c0-f0198b00fad6" xmlns:ns3="cc7c30c3-4b65-4cc6-b84c-43aad756a2f2" xmlns:ns4="5e13aadc-de86-43ee-b386-40c01ba74c80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="705beb6a12754410c5695455629349f7" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="2199b669-f139-4cad-81c0-f0198b00fad6"/>
+    <xsd:import namespace="cc7c30c3-4b65-4cc6-b84c-43aad756a2f2"/>
+    <xsd:import namespace="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2199b669-f139-4cad-81c0-f0198b00fad6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c0f44cca-6aff-4d49-827c-e4b3bc2e3f13" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cc7c30c3-4b65-4cc6-b84c-43aad756a2f2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5e13aadc-de86-43ee-b386-40c01ba74c80" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e6604573-ec2e-48b5-9821-b92072da312c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="cc7c30c3-4b65-4cc6-b84c-43aad756a2f2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4F1E04-D26F-4971-9D7C-5B9A939A9DF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2199b669-f139-4cad-81c0-f0198b00fad6"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6ECB3EF-B2E0-4D7E-BF48-BE0711D04338}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2199b669-f139-4cad-81c0-f0198b00fad6"/>
+    <ds:schemaRef ds:uri="cc7c30c3-4b65-4cc6-b84c-43aad756a2f2"/>
+    <ds:schemaRef ds:uri="5e13aadc-de86-43ee-b386-40c01ba74c80"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49F78637-B4C6-4CDA-A05F-EEA0E3FAA59F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>